<commit_message>
add ble andd ele
</commit_message>
<xml_diff>
--- a/hdyl/docs/BLE/协议.xlsx
+++ b/hdyl/docs/BLE/协议.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>数据头</t>
   </si>
@@ -36,6 +36,12 @@
     <t>命令</t>
   </si>
   <si>
+    <t>0x5b</t>
+  </si>
+  <si>
+    <t>配对指示</t>
+  </si>
+  <si>
     <t>0x5a</t>
   </si>
   <si>
@@ -52,6 +58,18 @@
   </si>
   <si>
     <t>0xfe</t>
+  </si>
+  <si>
+    <t>控制逻辑</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 建立连接后，主机发握手信号给从机，主从机检测到mac地址或者握手信号不对自动断开连接</t>
+  </si>
+  <si>
+    <t>握手成功后，如果从机震动开关规定时间内有振动则进行测量，否则不进行测量</t>
+  </si>
+  <si>
+    <t>主机按钮长按开关机，短按配对</t>
   </si>
 </sst>
 </file>
@@ -59,12 +77,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,21 +93,105 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -102,47 +204,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -154,71 +228,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,43 +244,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,31 +400,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,103 +418,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,6 +435,41 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -443,16 +489,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -489,188 +535,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1026,10 +1037,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:F11"/>
+  <dimension ref="B1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1075,19 +1086,45 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:2">
+    <row r="8" spans="2:3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="10" spans="2:2">
-      <c r="B10" t="s">
-        <v>0</v>
+    <row r="9" spans="2:2">
+      <c r="B9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>11</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3">
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>